<commit_message>
working txt translating agent for pptx, docx, xlsx, pdf
</commit_message>
<xml_diff>
--- a/backend/esempio.xlsx
+++ b/backend/esempio.xlsx
@@ -431,14 +431,14 @@
     <row r="2">
       <c r="B2" t="inlineStr">
         <is>
-          <t>LangChain può leggere anche file Excel.</t>
+          <t>Gemini può leggere anche file Excel.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="C3" t="inlineStr">
         <is>
-          <t>Questa è la cella C3 e contiene informazioni utili per il riassunto del foglio di calcolo. Lo scopo è testare l'estrazione da diverse celle.</t>
+          <t>Questa è la cella C3 e contiene informazioni utili per il riassunto del foglio di calcolo.</t>
         </is>
       </c>
     </row>

</xml_diff>